<commit_message>
isa pegou função validacao resposta
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEC84B05-0B73-4DC0-9137-0EC177A4524A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AEF0CA-11F0-4A68-8ED2-D166AFCB07A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>validação_Nome_de_Pessoa()</t>
   </si>
   <si>
-    <t>Em análise</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">As respostas da categoria “nome de pessoa” devem ser de uma só palavra. Apenas o </t>
     </r>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Concluído</t>
+  </si>
+  <si>
+    <t>isa</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +330,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -395,94 +401,106 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,200 +839,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="E1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="E2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="E2" s="31" t="s">
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="30" t="s">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="E4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="32"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="18"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="20"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="34"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="36"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="E4" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="28"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="20"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="20"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="23"/>
-      <c r="F12" s="32"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="23"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="22"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="23"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="24"/>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="25"/>
-    </row>
-    <row r="22" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Coloquei meu nome em contar_caractere()
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AEF0CA-11F0-4A68-8ED2-D166AFCB07A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDCFD42-3192-4B91-A5FE-F39DB9F4114F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Funcões</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>isa</t>
+  </si>
+  <si>
+    <t>Matheus</t>
   </si>
 </sst>
 </file>
@@ -431,9 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,13 +444,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -462,6 +465,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -489,16 +498,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -527,7 +530,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -825,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,26 +842,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="E1" s="21" t="s">
         <v>28</v>
       </c>
       <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="E2" s="16" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="E2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -870,33 +873,33 @@
       <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="E4" s="16" t="s">
+      <c r="C4" s="34"/>
+      <c r="E4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="32"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="32"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="34"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -908,34 +911,34 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="35"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="35"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="20"/>
-      <c r="F12" s="17"/>
+      <c r="C12" s="25"/>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -953,34 +956,34 @@
       <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="20"/>
+      <c r="C15" s="25"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="17"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="19"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="35"/>
+      <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -997,7 +1000,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="36"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1006,7 +1009,9 @@
       <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="36" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1030,7 +1035,7 @@
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="2"/>

</xml_diff>

<commit_message>
matheus na funcao validar_jogadores
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3D7FA9-108A-4408-8DF0-D58A78D33A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FEFA42-1B9D-48C9-9A76-0E02E6B7CD48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Funcões</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>isa</t>
+  </si>
+  <si>
+    <t>matheus</t>
   </si>
 </sst>
 </file>
@@ -444,6 +447,18 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,22 +498,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -527,7 +530,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -825,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,22 +842,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="E1" s="18" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="E2" s="15" t="s">
         <v>29</v>
       </c>
@@ -876,27 +879,29 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="31"/>
+      <c r="C4" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="E4" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="36"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -908,33 +913,33 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="25"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="32"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="32"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="35"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="35"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="22"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="26"/>
       <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,40 +952,40 @@
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="25"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="19" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="20"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="35"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1006,7 +1011,7 @@
       <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="18" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
terminei função de sortear categoria
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FEFA42-1B9D-48C9-9A76-0E02E6B7CD48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF4199F-9BA0-46E9-8644-173A44BAC416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Funcões</t>
   </si>
@@ -340,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -394,6 +394,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -498,12 +509,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +539,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -829,7 +838,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +894,7 @@
       <c r="B4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="15" t="s">
@@ -896,12 +905,12 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="33"/>
-      <c r="C5" s="36"/>
+      <c r="C5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="33"/>
-      <c r="C6" s="36"/>
+      <c r="C6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -919,27 +928,29 @@
       <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="27"/>
-      <c r="C9" s="35"/>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="27"/>
-      <c r="C10" s="35"/>
+      <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
       <c r="B11" s="27"/>
-      <c r="C11" s="35"/>
+      <c r="C11" s="20"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="24"/>
-      <c r="C12" s="26"/>
+      <c r="C12" s="21"/>
       <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -950,6 +961,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -993,6 +1005,7 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="10"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">

</xml_diff>

<commit_message>
estilizei os campos do formulário
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF4199F-9BA0-46E9-8644-173A44BAC416}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749CE683-27E1-42C1-A54C-E7FE36FE2721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Funcões</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>matheus</t>
+  </si>
+  <si>
+    <t>Matheus</t>
   </si>
 </sst>
 </file>
@@ -442,9 +445,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,6 +461,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,7 +513,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +542,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -837,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,10 +870,10 @@
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -882,7 +885,7 @@
       <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="6"/>
@@ -897,10 +900,10 @@
       <c r="C4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
@@ -951,7 +954,7 @@
       <c r="A12" s="30"/>
       <c r="B12" s="24"/>
       <c r="C12" s="21"/>
-      <c r="F12" s="16"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -961,7 +964,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="16"/>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -987,7 +990,7 @@
       <c r="C16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
@@ -1004,8 +1007,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="36"/>
+      <c r="C19" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1015,7 +1020,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="17"/>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1024,7 +1029,7 @@
       <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1036,7 +1041,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="16"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1051,7 +1056,7 @@
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="2"/>

</xml_diff>

<commit_message>
matheus começar a fazer funçao de marcar tempo
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749CE683-27E1-42C1-A54C-E7FE36FE2721}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503AAA1D-4579-4E19-848E-6DF4837707D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Funcões</t>
   </si>
@@ -462,6 +462,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,12 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -513,7 +510,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -841,7 +841,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C16" sqref="C16:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,22 +854,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="E1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="E2" s="14" t="s">
         <v>29</v>
       </c>
@@ -891,13 +891,13 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="14" t="s">
@@ -906,14 +906,14 @@
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="35"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="34"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -925,35 +925,35 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="20"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="21"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="22"/>
       <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,47 +967,49 @@
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="35" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="26"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="20" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="21"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="22"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="19" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="18"/>

</xml_diff>

<commit_message>
alocação dinâmica nas funções
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503AAA1D-4579-4E19-848E-6DF4837707D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D5267-3058-46C6-B0BD-6601B1A39D95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Funcões</t>
   </si>
@@ -418,12 +418,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,9 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -458,11 +452,11 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -507,15 +501,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,7 +544,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -841,79 +843,79 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="110.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="38" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="E1" s="23" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="E1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="23"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="E2" s="14" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="E2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="34"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="37"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="34"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="37"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -922,113 +924,119 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="33" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="21"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="21"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="21"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="22"/>
-      <c r="F12" s="15"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="36"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="36"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="35"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="19"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="22"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="19" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="16"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="17" t="s">
@@ -1039,29 +1047,29 @@
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="15"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="32"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
funcao marcar tempo concluida
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D5267-3058-46C6-B0BD-6601B1A39D95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48AB50-D067-4995-BBA3-E1ED0632C2E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Funcões</t>
   </si>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,6 +459,14 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,23 +509,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +538,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -842,36 +836,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="110.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="38" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="21" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="21"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
       <c r="E2" s="12" t="s">
         <v>29</v>
       </c>
@@ -893,13 +887,13 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -908,14 +902,14 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="36"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -924,42 +918,42 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="36"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="20"/>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -969,48 +963,48 @@
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="19" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="35"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="24"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="19"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1029,7 +1023,7 @@
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="32"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,7 +1044,7 @@
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="32"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1060,7 +1054,7 @@
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="32"/>
+      <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1069,7 +1063,9 @@
       <c r="B24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="32"/>
+      <c r="C24" s="19" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
fiz sortear letra e sortear jogadores
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48AB50-D067-4995-BBA3-E1ED0632C2E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE12ADAE-E93A-4FEA-8962-CA201AEA9321}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -467,6 +467,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -538,7 +541,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -836,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,22 +853,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="E1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="25"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
       <c r="E2" s="12" t="s">
         <v>29</v>
       </c>
@@ -887,13 +890,13 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -902,14 +905,14 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="36"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -918,41 +921,41 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="23"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="24"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="23"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="24"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="20"/>
       <c r="F12" s="13"/>
     </row>
@@ -963,48 +966,48 @@
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="25"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="24"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="24"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="25"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">

</xml_diff>

<commit_message>
adicionei mais uma função
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE12ADAE-E93A-4FEA-8962-CA201AEA9321}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09487F5-FA8F-4D5F-996C-2EB4CC42A989}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Funcões</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Matheus</t>
+  </si>
+  <si>
+    <t>pontuacao_Resposta()</t>
+  </si>
+  <si>
+    <t>Soma da pontuação de todas as rodadas</t>
   </si>
 </sst>
 </file>
@@ -418,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -470,6 +476,12 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,6 +526,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,22 +869,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="E1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="26"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
       <c r="E2" s="12" t="s">
         <v>29</v>
       </c>
@@ -890,13 +906,13 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="39" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -905,14 +921,14 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="39"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -926,36 +942,36 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="25" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="26"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="20"/>
       <c r="F12" s="13"/>
     </row>
@@ -972,42 +988,42 @@
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="25"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="24"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="26"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="27"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1041,10 +1057,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="18"/>
@@ -1069,6 +1085,15 @@
       <c r="C24" s="19" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
fiz as funcoes limite_excedido e somatorio_tempo
</commit_message>
<xml_diff>
--- a/Trabalho_Intermediario.xlsx
+++ b/Trabalho_Intermediario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gatita\Desktop\jogo-amedanha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\Desktop\jogo-amedanha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09487F5-FA8F-4D5F-996C-2EB4CC42A989}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E2FA8-CEDE-473F-9CAB-191F7A49C2E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19740" windowHeight="11760" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6ADE7DC6-245E-4865-B772-D66B5C3BB650}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -468,9 +468,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -482,54 +479,57 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,7 +557,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -855,36 +855,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF691E1F-E154-4635-8DFB-BE3A7491504D}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="110.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="20" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="E1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="28"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="E2" s="12" t="s">
         <v>29</v>
       </c>
@@ -906,13 +906,13 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="41" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -921,14 +921,14 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="41"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="39"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="41"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -937,42 +937,42 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="26"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="28"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="20"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="20"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="19"/>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -982,48 +982,48 @@
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="27" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1057,10 +1057,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="26" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="18"/>
@@ -1082,18 +1082,18 @@
       <c r="B24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="40"/>
+      <c r="C25" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>